<commit_message>
Added scanning task description, creating new file if doesn't exist and createNewSheet method
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip\IdeaProjects\Work_Time_Track_Automation_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BB836E-04B5-48FC-8CB7-624E70891A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2083A7-9757-4D58-9183-9293F3DAF009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="5540" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="5540" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,33 +25,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Start</t>
   </si>
   <si>
-    <t>Finish</t>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Task Description</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>2021-AUGUST-25 15:40:38</t>
-  </si>
-  <si>
-    <t>2021-AUGUST-25 15:40:45</t>
-  </si>
-  <si>
-    <t>0:00:06</t>
-  </si>
-  <si>
-    <t>2021-AUGUST-25 15:44:19</t>
-  </si>
-  <si>
-    <t>2021-AUGUST-25 17:45:19</t>
-  </si>
-  <si>
-    <t>2:00:59</t>
+    <t>2021-08-26 13:11:14</t>
+  </si>
+  <si>
+    <t>jakiś Task</t>
+  </si>
+  <si>
+    <t>0:00:00</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:12:42</t>
+  </si>
+  <si>
+    <t>sffasfsf</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:13:36</t>
+  </si>
+  <si>
+    <t>rgdfgfdsg</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:15:48</t>
+  </si>
+  <si>
+    <t>wdfgdfg</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:21:47</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:22:10</t>
+  </si>
+  <si>
+    <t>adgdfga</t>
+  </si>
+  <si>
+    <t>0:00:23</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:25:31</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:25:33</t>
+  </si>
+  <si>
+    <t>jakiś opis</t>
+  </si>
+  <si>
+    <t>0:00:01</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:30:35</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:30:47</t>
+  </si>
+  <si>
+    <t>przykładowy opis</t>
+  </si>
+  <si>
+    <t>0:00:11</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:40:48</t>
+  </si>
+  <si>
+    <t>2021-08-26 13:40:53</t>
+  </si>
+  <si>
+    <t>costam</t>
+  </si>
+  <si>
+    <t>0:00:04</t>
   </si>
 </sst>
 </file>
@@ -370,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,10 +448,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -399,16 +462,106 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>